<commit_message>
amended code on Sept 28
</commit_message>
<xml_diff>
--- a/20220914_cleaned_data.xlsx
+++ b/20220914_cleaned_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10814"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelmartin/Dropbox/Research/Papers/Papers in Progress/Belt Study Papers/Hip Hinge/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joelmartin/belt_study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A98C0986-521E-2842-8056-C4516D167E4B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BACABEB-D7BE-7A4B-9C91-3B28E94EB783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22960" yWindow="140" windowWidth="34340" windowHeight="13320" activeTab="1" xr2:uid="{9CA849AB-732E-D747-A1FB-DEBE88E38172}"/>
+    <workbookView xWindow="-28800" yWindow="140" windowWidth="28800" windowHeight="13320" xr2:uid="{9CA849AB-732E-D747-A1FB-DEBE88E38172}"/>
   </bookViews>
   <sheets>
     <sheet name="cleaned_data" sheetId="1" r:id="rId1"/>
@@ -643,7 +643,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6FD82547-AD89-0D4E-AA93-B3B5E61CA145}">
   <dimension ref="A1:CJ97"/>
   <sheetViews>
-    <sheetView topLeftCell="BN84" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="BN1" workbookViewId="0">
       <selection activeCell="CJ97" sqref="BU1:CJ97"/>
     </sheetView>
   </sheetViews>
@@ -26745,7 +26745,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8769DAA0-D3EA-734F-86B2-E7C4976EFD0A}">
   <dimension ref="A1:CP97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AQ1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="BA2" sqref="BA2:BO97"/>
     </sheetView>
   </sheetViews>

</xml_diff>